<commit_message>
changed gui to match tutorial 3
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="72">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,6 +171,66 @@
   </si>
   <si>
     <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;m&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;minute&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hour&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hour&gt;:&lt;minu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;hour&gt;:&lt;minute&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1688,7 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -1645,7 +1705,143 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating text from Model
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="52">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
   </si>
 </sst>
 </file>
@@ -1429,7 +1432,9 @@
         <v>17</v>
       </c>
       <c r="G5"/>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
       <c r="I5"/>
       <c r="K5" s="7" t="s">
         <v>1</v>
@@ -1617,7 +1622,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>

</xml_diff>